<commit_message>
euro 2024 group c 0-0
</commit_message>
<xml_diff>
--- a/data/out/wiki/men/uefa/eu/third_teams_df_eu_uefa.xlsx
+++ b/data/out/wiki/men/uefa/eu/third_teams_df_eu_uefa.xlsx
@@ -7420,27 +7420,27 @@
       </c>
       <c r="K91" t="inlineStr">
         <is>
-          <t>['Slovakia', 4, 0, 3]</t>
+          <t>['Belgium', 3, 1, 2]</t>
         </is>
       </c>
       <c r="L91" t="inlineStr">
         <is>
-          <t>['Georgia', 4, 0, 4]</t>
+          <t>['Czech Republic', 1, -1, 2]</t>
         </is>
       </c>
       <c r="M91" t="inlineStr">
         <is>
-          <t>['Netherlands', 'Georgia', 'Slovakia', 'Slovenia']</t>
+          <t>['Netherlands', 'Belgium', 'Slovenia', 'Hungary']</t>
         </is>
       </c>
       <c r="N91" t="inlineStr">
         <is>
-          <t>['Hungary', 'Croatia']</t>
+          <t>['Croatia', 'Czech Republic']</t>
         </is>
       </c>
       <c r="O91" t="inlineStr">
         <is>
-          <t>['Georgia', 'Netherlands']</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="P91" t="n">
@@ -7487,7 +7487,7 @@
       </c>
       <c r="I92" t="inlineStr">
         <is>
-          <t>['Slovenia', 2, 0, 2]</t>
+          <t>['Slovenia', 3, 0, 2]</t>
         </is>
       </c>
       <c r="J92" t="inlineStr">
@@ -7507,7 +7507,7 @@
       </c>
       <c r="M92" t="inlineStr">
         <is>
-          <t>['Belgium', 'Netherlands', 'Hungary', 'Slovenia']</t>
+          <t>['Belgium', 'Netherlands', 'Slovenia', 'Hungary']</t>
         </is>
       </c>
       <c r="N92" t="inlineStr">
@@ -7564,7 +7564,7 @@
       </c>
       <c r="I93" t="inlineStr">
         <is>
-          <t>['Slovenia', 2, 0, 2]</t>
+          <t>['Slovenia', 3, 0, 2]</t>
         </is>
       </c>
       <c r="J93" t="inlineStr">
@@ -7584,7 +7584,7 @@
       </c>
       <c r="M93" t="inlineStr">
         <is>
-          <t>['Netherlands', 'Ukraine', 'Hungary', 'Slovenia']</t>
+          <t>['Netherlands', 'Ukraine', 'Slovenia', 'Hungary']</t>
         </is>
       </c>
       <c r="N93" t="inlineStr">
@@ -7641,7 +7641,7 @@
       </c>
       <c r="I94" t="inlineStr">
         <is>
-          <t>['Slovenia', 2, 0, 2]</t>
+          <t>['Slovenia', 3, 0, 2]</t>
         </is>
       </c>
       <c r="J94" t="inlineStr">
@@ -7661,7 +7661,7 @@
       </c>
       <c r="M94" t="inlineStr">
         <is>
-          <t>['Netherlands', 'Slovakia', 'Hungary', 'Slovenia']</t>
+          <t>['Netherlands', 'Slovakia', 'Slovenia', 'Hungary']</t>
         </is>
       </c>
       <c r="N94" t="inlineStr">
@@ -7718,7 +7718,7 @@
       </c>
       <c r="I95" t="inlineStr">
         <is>
-          <t>['Slovenia', 2, 0, 2]</t>
+          <t>['Slovenia', 3, 0, 2]</t>
         </is>
       </c>
       <c r="J95" t="inlineStr">
@@ -7738,7 +7738,7 @@
       </c>
       <c r="M95" t="inlineStr">
         <is>
-          <t>['Netherlands', 'Slovakia', 'Hungary', 'Slovenia']</t>
+          <t>['Netherlands', 'Slovakia', 'Slovenia', 'Hungary']</t>
         </is>
       </c>
       <c r="N95" t="inlineStr">
@@ -7795,7 +7795,7 @@
       </c>
       <c r="I96" t="inlineStr">
         <is>
-          <t>['Slovenia', 2, 0, 2]</t>
+          <t>['Slovenia', 3, 0, 2]</t>
         </is>
       </c>
       <c r="J96" t="inlineStr">
@@ -7815,12 +7815,12 @@
       </c>
       <c r="M96" t="inlineStr">
         <is>
-          <t>['Netherlands', 'Slovakia', 'Georgia', 'Hungary']</t>
+          <t>['Netherlands', 'Slovakia', 'Georgia', 'Slovenia']</t>
         </is>
       </c>
       <c r="N96" t="inlineStr">
         <is>
-          <t>['Slovenia', 'Croatia']</t>
+          <t>['Hungary', 'Croatia']</t>
         </is>
       </c>
       <c r="O96" t="inlineStr">
@@ -7872,7 +7872,7 @@
       </c>
       <c r="I97" t="inlineStr">
         <is>
-          <t>['Slovenia', 2, 0, 2]</t>
+          <t>['Slovenia', 3, 0, 2]</t>
         </is>
       </c>
       <c r="J97" t="inlineStr">
@@ -7892,12 +7892,12 @@
       </c>
       <c r="M97" t="inlineStr">
         <is>
-          <t>['Netherlands', 'Slovakia', 'Georgia', 'Hungary']</t>
+          <t>['Netherlands', 'Slovakia', 'Georgia', 'Slovenia']</t>
         </is>
       </c>
       <c r="N97" t="inlineStr">
         <is>
-          <t>['Slovenia', 'Croatia']</t>
+          <t>['Hungary', 'Croatia']</t>
         </is>
       </c>
       <c r="O97" t="inlineStr">
@@ -7949,7 +7949,7 @@
       </c>
       <c r="I98" t="inlineStr">
         <is>
-          <t>['Slovenia', 2, 0, 2]</t>
+          <t>['Slovenia', 3, 0, 2]</t>
         </is>
       </c>
       <c r="J98" t="inlineStr">
@@ -7969,12 +7969,12 @@
       </c>
       <c r="M98" t="inlineStr">
         <is>
-          <t>['Netherlands', 'Georgia', 'Slovakia', 'Hungary']</t>
+          <t>['Netherlands', 'Georgia', 'Slovakia', 'Slovenia']</t>
         </is>
       </c>
       <c r="N98" t="inlineStr">
         <is>
-          <t>['Slovenia', 'Croatia']</t>
+          <t>['Hungary', 'Croatia']</t>
         </is>
       </c>
       <c r="O98" t="inlineStr">
@@ -8026,7 +8026,7 @@
       </c>
       <c r="I99" t="inlineStr">
         <is>
-          <t>['Slovenia', 2, 0, 2]</t>
+          <t>['Slovenia', 3, 0, 2]</t>
         </is>
       </c>
       <c r="J99" t="inlineStr">
@@ -8046,12 +8046,12 @@
       </c>
       <c r="M99" t="inlineStr">
         <is>
-          <t>['Netherlands', 'Georgia', 'Slovakia', 'Hungary']</t>
+          <t>['Netherlands', 'Georgia', 'Slovakia', 'Slovenia']</t>
         </is>
       </c>
       <c r="N99" t="inlineStr">
         <is>
-          <t>['Slovenia', 'Croatia']</t>
+          <t>['Hungary', 'Croatia']</t>
         </is>
       </c>
       <c r="O99" t="inlineStr">
@@ -8103,7 +8103,7 @@
       </c>
       <c r="I100" t="inlineStr">
         <is>
-          <t>['Slovenia', 2, 0, 2]</t>
+          <t>['Slovenia', 3, 0, 2]</t>
         </is>
       </c>
       <c r="J100" t="inlineStr">
@@ -8123,12 +8123,12 @@
       </c>
       <c r="M100" t="inlineStr">
         <is>
-          <t>['Netherlands', 'Georgia', 'Slovakia', 'Hungary']</t>
+          <t>['Netherlands', 'Georgia', 'Slovakia', 'Slovenia']</t>
         </is>
       </c>
       <c r="N100" t="inlineStr">
         <is>
-          <t>['Slovenia', 'Croatia']</t>
+          <t>['Hungary', 'Croatia']</t>
         </is>
       </c>
       <c r="O100" t="inlineStr">

</xml_diff>